<commit_message>
Add Fuel Surcharge Page
</commit_message>
<xml_diff>
--- a/downloads/fuel_surcharge_tables.xlsx
+++ b/downloads/fuel_surcharge_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/callum.herries/Code/fuel/fuelsurcharges/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32089D9C-1CF9-214E-8533-46CA29E7EB65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FD5894-A4DA-F140-8151-2ED262A4D49D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18018,7 +18018,7 @@
   <dimension ref="A1:I1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A14"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>